<commit_message>
level3 update - new puzzle area
</commit_message>
<xml_diff>
--- a/res/levels/lvl3/map.xlsx
+++ b/res/levels/lvl3/map.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Software\Programing_Projects\Java\unnamedGame\res\levels\lvl3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Software\Programing_Projects\Java\LittleCatGoesTheKnowledgePath\res\levels\lvl3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3A61E23-6604-4AA8-A59D-03CFEF024822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD513D1-3A7E-49F0-8154-AB613A46E8FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14520" windowHeight="15585" xr2:uid="{A5438383-251D-4F5B-B97C-6B89082557F3}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{A5438383-251D-4F5B-B97C-6B89082557F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -420,8 +420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC41A6BD-6C1D-4B00-B11B-8117918BDFDE}">
   <dimension ref="A1:AP129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66:AP129"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L63" sqref="L63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +537,7 @@
         <v>4</v>
       </c>
       <c r="AJ1" s="1">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AK1" s="1">
         <v>4</v>
@@ -665,7 +665,7 @@
         <v>4</v>
       </c>
       <c r="AJ2" s="1">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AK2" s="1">
         <v>4</v>
@@ -793,7 +793,7 @@
         <v>4</v>
       </c>
       <c r="AJ3" s="1">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AK3" s="1">
         <v>4</v>
@@ -921,7 +921,7 @@
         <v>4</v>
       </c>
       <c r="AJ4" s="1">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AK4" s="1">
         <v>4</v>
@@ -1049,7 +1049,7 @@
         <v>4</v>
       </c>
       <c r="AJ5" s="1">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AK5" s="1">
         <v>13</v>
@@ -1668,7 +1668,7 @@
         <v>4</v>
       </c>
       <c r="AC10" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AD10" s="1">
         <v>5</v>
@@ -2195,7 +2195,7 @@
         <v>6</v>
       </c>
       <c r="AH14" s="1">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AI14" s="1">
         <v>0</v>
@@ -2207,7 +2207,7 @@
         <v>0</v>
       </c>
       <c r="AL14" s="1">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AM14" s="1">
         <v>6</v>
@@ -2323,7 +2323,7 @@
         <v>6</v>
       </c>
       <c r="AH15" s="1">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AI15" s="1">
         <v>0</v>
@@ -2335,7 +2335,7 @@
         <v>0</v>
       </c>
       <c r="AL15" s="1">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AM15" s="1">
         <v>6</v>
@@ -2451,7 +2451,7 @@
         <v>6</v>
       </c>
       <c r="AH16" s="1">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AI16" s="1">
         <v>0</v>
@@ -2463,7 +2463,7 @@
         <v>0</v>
       </c>
       <c r="AL16" s="1">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AM16" s="1">
         <v>6</v>
@@ -2579,7 +2579,7 @@
         <v>6</v>
       </c>
       <c r="AH17" s="1">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AI17" s="1">
         <v>0</v>
@@ -2591,7 +2591,7 @@
         <v>0</v>
       </c>
       <c r="AL17" s="1">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AM17" s="1">
         <v>6</v>
@@ -3397,7 +3397,7 @@
         <v>0</v>
       </c>
       <c r="H24" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="I24" s="1">
         <v>0</v>
@@ -4984,7 +4984,7 @@
         <v>0</v>
       </c>
       <c r="Y36" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="Z36" s="1">
         <v>0</v>
@@ -5115,10 +5115,10 @@
         <v>6</v>
       </c>
       <c r="Z37" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA37" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB37" s="1">
         <v>0</v>
@@ -5657,7 +5657,7 @@
         <v>0</v>
       </c>
       <c r="AJ41" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AK41" s="1">
         <v>0</v>
@@ -6044,7 +6044,7 @@
         <v>10</v>
       </c>
       <c r="AK44" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AL44" s="1">
         <v>0</v>
@@ -6169,7 +6169,7 @@
         <v>0</v>
       </c>
       <c r="AJ45" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AK45" s="1">
         <v>10</v>
@@ -6297,7 +6297,7 @@
         <v>0</v>
       </c>
       <c r="AJ46" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AK46" s="1">
         <v>10</v>
@@ -6428,7 +6428,7 @@
         <v>10</v>
       </c>
       <c r="AK47" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AL47" s="1">
         <v>0</v>
@@ -6681,7 +6681,7 @@
         <v>0</v>
       </c>
       <c r="AJ49" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AK49" s="1">
         <v>0</v>
@@ -6812,7 +6812,7 @@
         <v>7</v>
       </c>
       <c r="AK50" s="1">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AL50" s="1">
         <v>0</v>
@@ -6835,7 +6835,7 @@
         <v>0</v>
       </c>
       <c r="B51" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C51" s="1">
         <v>0</v>
@@ -6960,10 +6960,10 @@
     </row>
     <row r="52" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B52" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C52" s="1">
         <v>0</v>
@@ -7068,13 +7068,13 @@
         <v>0</v>
       </c>
       <c r="AK52" s="1">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AL52" s="1">
         <v>7</v>
       </c>
       <c r="AM52" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AN52" s="1">
         <v>0</v>
@@ -7088,10 +7088,10 @@
     </row>
     <row r="53" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B53" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C53" s="1">
         <v>0</v>
@@ -7121,31 +7121,31 @@
         <v>0</v>
       </c>
       <c r="L53" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M53" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="N53" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="O53" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="P53" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q53" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="R53" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="S53" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="T53" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="U53" s="1">
         <v>0</v>
@@ -7172,7 +7172,7 @@
         <v>0</v>
       </c>
       <c r="AC53" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="AD53" s="1">
         <v>0</v>
@@ -7219,7 +7219,7 @@
         <v>0</v>
       </c>
       <c r="B54" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C54" s="1">
         <v>0</v>
@@ -7249,10 +7249,10 @@
         <v>0</v>
       </c>
       <c r="L54" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M54" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N54" s="1">
         <v>0</v>
@@ -7270,10 +7270,10 @@
         <v>0</v>
       </c>
       <c r="S54" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T54" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="U54" s="1">
         <v>0</v>
@@ -7347,7 +7347,7 @@
         <v>0</v>
       </c>
       <c r="B55" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C55" s="1">
         <v>0</v>
@@ -7377,10 +7377,10 @@
         <v>0</v>
       </c>
       <c r="L55" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M55" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N55" s="1">
         <v>0</v>
@@ -7389,7 +7389,7 @@
         <v>0</v>
       </c>
       <c r="P55" s="1">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="Q55" s="1">
         <v>0</v>
@@ -7398,10 +7398,10 @@
         <v>0</v>
       </c>
       <c r="S55" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T55" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="U55" s="1">
         <v>0</v>
@@ -7475,7 +7475,7 @@
         <v>0</v>
       </c>
       <c r="B56" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C56" s="1">
         <v>0</v>
@@ -7505,31 +7505,31 @@
         <v>0</v>
       </c>
       <c r="L56" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M56" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="N56" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="O56" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="P56" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q56" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="R56" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="S56" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="T56" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="U56" s="1">
         <v>0</v>
@@ -7633,7 +7633,7 @@
         <v>0</v>
       </c>
       <c r="L57" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M57" s="1">
         <v>0</v>
@@ -7657,7 +7657,7 @@
         <v>0</v>
       </c>
       <c r="T57" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="U57" s="1">
         <v>0</v>
@@ -7761,13 +7761,13 @@
         <v>0</v>
       </c>
       <c r="L58" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M58" s="1">
         <v>0</v>
       </c>
       <c r="N58" s="1">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O58" s="1">
         <v>0</v>
@@ -7779,13 +7779,13 @@
         <v>0</v>
       </c>
       <c r="R58" s="1">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="S58" s="1">
         <v>0</v>
       </c>
       <c r="T58" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="U58" s="1">
         <v>0</v>
@@ -7889,31 +7889,31 @@
         <v>0</v>
       </c>
       <c r="L59" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M59" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="N59" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="O59" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="P59" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="Q59" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="R59" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="S59" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="T59" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="U59" s="1">
         <v>0</v>
@@ -8020,7 +8020,7 @@
         <v>0</v>
       </c>
       <c r="M60" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N60" s="1">
         <v>0</v>
@@ -8038,7 +8038,7 @@
         <v>0</v>
       </c>
       <c r="S60" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T60" s="1">
         <v>0</v>
@@ -8142,37 +8142,37 @@
         <v>0</v>
       </c>
       <c r="K61" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L61" s="1">
         <v>0</v>
       </c>
       <c r="M61" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N61" s="1">
         <v>0</v>
       </c>
       <c r="O61" s="1">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="P61" s="1">
         <v>0</v>
       </c>
       <c r="Q61" s="1">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="R61" s="1">
         <v>0</v>
       </c>
       <c r="S61" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T61" s="1">
         <v>0</v>
       </c>
       <c r="U61" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="V61" s="1">
         <v>0</v>
@@ -8264,52 +8264,52 @@
         <v>0</v>
       </c>
       <c r="I62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L62" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M62" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="N62" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="O62" s="1">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="P62" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q62" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="R62" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="S62" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="T62" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="U62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y62" s="1">
         <v>0</v>
@@ -8392,52 +8392,52 @@
         <v>1</v>
       </c>
       <c r="I63" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J63" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K63" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L63" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M63" s="1">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="N63" s="1">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="O63" s="1">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="P63" s="1">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="Q63" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="R63" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S63" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T63" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U63" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V63" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W63" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X63" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y63" s="1">
         <v>1</v>
@@ -8529,10 +8529,10 @@
         <v>2</v>
       </c>
       <c r="L64" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M64" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N64" s="1">
         <v>7</v>
@@ -8544,16 +8544,16 @@
         <v>7</v>
       </c>
       <c r="Q64" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R64" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S64" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="T64" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="U64" s="1">
         <v>2</v>
@@ -8729,7 +8729,7 @@
         <v>1</v>
       </c>
       <c r="AJ66" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AK66" s="1">
         <v>1</v>
@@ -8857,7 +8857,7 @@
         <v>1</v>
       </c>
       <c r="AJ67" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AK67" s="1">
         <v>1</v>
@@ -8985,7 +8985,7 @@
         <v>1</v>
       </c>
       <c r="AJ68" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AK68" s="1">
         <v>1</v>
@@ -9113,7 +9113,7 @@
         <v>1</v>
       </c>
       <c r="AJ69" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AK69" s="1">
         <v>1</v>
@@ -9241,7 +9241,7 @@
         <v>1</v>
       </c>
       <c r="AJ70" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AK70" s="1">
         <v>1</v>
@@ -9860,7 +9860,7 @@
         <v>1</v>
       </c>
       <c r="AC75" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD75" s="1">
         <v>1</v>
@@ -10387,7 +10387,7 @@
         <v>1</v>
       </c>
       <c r="AH79" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AI79" s="1">
         <v>0</v>
@@ -10399,7 +10399,7 @@
         <v>0</v>
       </c>
       <c r="AL79" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AM79" s="1">
         <v>1</v>
@@ -10515,7 +10515,7 @@
         <v>1</v>
       </c>
       <c r="AH80" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AI80" s="1">
         <v>0</v>
@@ -10527,7 +10527,7 @@
         <v>0</v>
       </c>
       <c r="AL80" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AM80" s="1">
         <v>1</v>
@@ -10643,7 +10643,7 @@
         <v>1</v>
       </c>
       <c r="AH81" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AI81" s="1">
         <v>0</v>
@@ -10655,7 +10655,7 @@
         <v>0</v>
       </c>
       <c r="AL81" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AM81" s="1">
         <v>1</v>
@@ -10771,7 +10771,7 @@
         <v>1</v>
       </c>
       <c r="AH82" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AI82" s="1">
         <v>0</v>
@@ -10783,7 +10783,7 @@
         <v>0</v>
       </c>
       <c r="AL82" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AM82" s="1">
         <v>1</v>
@@ -13307,10 +13307,10 @@
         <v>1</v>
       </c>
       <c r="Z102" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA102" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB102" s="1">
         <v>0</v>
@@ -13849,7 +13849,7 @@
         <v>0</v>
       </c>
       <c r="AJ106" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AK106" s="1">
         <v>0</v>
@@ -14236,7 +14236,7 @@
         <v>3</v>
       </c>
       <c r="AK109" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL109" s="1">
         <v>0</v>
@@ -14361,7 +14361,7 @@
         <v>0</v>
       </c>
       <c r="AJ110" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AK110" s="1">
         <v>3</v>
@@ -14489,7 +14489,7 @@
         <v>0</v>
       </c>
       <c r="AJ111" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK111" s="1">
         <v>3</v>
@@ -14620,7 +14620,7 @@
         <v>3</v>
       </c>
       <c r="AK112" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL112" s="1">
         <v>0</v>
@@ -14873,7 +14873,7 @@
         <v>0</v>
       </c>
       <c r="AJ114" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AK114" s="1">
         <v>0</v>
@@ -15004,7 +15004,7 @@
         <v>1</v>
       </c>
       <c r="AK115" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL115" s="1">
         <v>0</v>
@@ -15027,7 +15027,7 @@
         <v>0</v>
       </c>
       <c r="B116" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C116" s="1">
         <v>0</v>
@@ -15152,10 +15152,10 @@
     </row>
     <row r="117" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B117" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C117" s="1">
         <v>0</v>
@@ -15260,13 +15260,13 @@
         <v>0</v>
       </c>
       <c r="AK117" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL117" s="1">
         <v>1</v>
       </c>
       <c r="AM117" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN117" s="1">
         <v>0</v>
@@ -15280,10 +15280,10 @@
     </row>
     <row r="118" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B118" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C118" s="1">
         <v>0</v>
@@ -15313,31 +15313,31 @@
         <v>0</v>
       </c>
       <c r="L118" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M118" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N118" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O118" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P118" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q118" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R118" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S118" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T118" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U118" s="1">
         <v>0</v>
@@ -15411,7 +15411,7 @@
         <v>0</v>
       </c>
       <c r="B119" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C119" s="1">
         <v>0</v>
@@ -15441,10 +15441,10 @@
         <v>0</v>
       </c>
       <c r="L119" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M119" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N119" s="1">
         <v>0</v>
@@ -15462,10 +15462,10 @@
         <v>0</v>
       </c>
       <c r="S119" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T119" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U119" s="1">
         <v>0</v>
@@ -15539,7 +15539,7 @@
         <v>0</v>
       </c>
       <c r="B120" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C120" s="1">
         <v>0</v>
@@ -15569,10 +15569,10 @@
         <v>0</v>
       </c>
       <c r="L120" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M120" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N120" s="1">
         <v>0</v>
@@ -15590,10 +15590,10 @@
         <v>0</v>
       </c>
       <c r="S120" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T120" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U120" s="1">
         <v>0</v>
@@ -15667,7 +15667,7 @@
         <v>0</v>
       </c>
       <c r="B121" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C121" s="1">
         <v>0</v>
@@ -15697,31 +15697,31 @@
         <v>0</v>
       </c>
       <c r="L121" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M121" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N121" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O121" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P121" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q121" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R121" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S121" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T121" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U121" s="1">
         <v>0</v>
@@ -15825,7 +15825,7 @@
         <v>0</v>
       </c>
       <c r="L122" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M122" s="1">
         <v>0</v>
@@ -15849,7 +15849,7 @@
         <v>0</v>
       </c>
       <c r="T122" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U122" s="1">
         <v>0</v>
@@ -15953,13 +15953,13 @@
         <v>0</v>
       </c>
       <c r="L123" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M123" s="1">
         <v>0</v>
       </c>
       <c r="N123" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O123" s="1">
         <v>0</v>
@@ -15971,13 +15971,13 @@
         <v>0</v>
       </c>
       <c r="R123" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S123" s="1">
         <v>0</v>
       </c>
       <c r="T123" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U123" s="1">
         <v>0</v>
@@ -16081,31 +16081,31 @@
         <v>0</v>
       </c>
       <c r="L124" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M124" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N124" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O124" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P124" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q124" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R124" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S124" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T124" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U124" s="1">
         <v>0</v>
@@ -16212,7 +16212,7 @@
         <v>0</v>
       </c>
       <c r="M125" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N125" s="1">
         <v>0</v>
@@ -16230,7 +16230,7 @@
         <v>0</v>
       </c>
       <c r="S125" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T125" s="1">
         <v>0</v>
@@ -16340,7 +16340,7 @@
         <v>0</v>
       </c>
       <c r="M126" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N126" s="1">
         <v>0</v>
@@ -16358,7 +16358,7 @@
         <v>0</v>
       </c>
       <c r="S126" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T126" s="1">
         <v>0</v>
@@ -16456,52 +16456,52 @@
         <v>0</v>
       </c>
       <c r="I127" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J127" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K127" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L127" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M127" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N127" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O127" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P127" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q127" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R127" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S127" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T127" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U127" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V127" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W127" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X127" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y127" s="1">
         <v>0</v>
@@ -16593,31 +16593,31 @@
         <v>1</v>
       </c>
       <c r="L128" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M128" s="1">
         <v>1</v>
       </c>
       <c r="N128" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O128" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P128" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q128" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R128" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S128" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T128" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U128" s="1">
         <v>1</v>

</xml_diff>